<commit_message>
Direction has been indicated on the map
</commit_message>
<xml_diff>
--- a/Honeymoon_Locations.xlsx
+++ b/Honeymoon_Locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HJ\Python\HoneyMoon_Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C22BEC-ACD0-400F-AFC6-9B1C3EDBA7D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6337605C-C67B-4BA0-A12B-B487C5207A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{5554A70D-75DD-49DE-8066-5822D9CA01A4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="60">
   <si>
     <t>위도</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -106,10 +106,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>액티비티</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>https://www.google.com/maps/place/%EC%9D%91%EA%B3%A0%EB%A1%B1%EA%B3%A0%EB%A1%9C+%EB%B6%84%ED%99%94%EA%B5%AC/@-3.3909797,35.3840207,10z/data=!4m6!3m5!1s0x1834764134612ca1:0x9597bd98b8bee7bc!8m2!3d-3.0653671!4d35.3817603!16zL20vMDRrM2M0?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -194,10 +190,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://www.google.com/maps/place/%EB%82%98%EB%AF%B8%EB%B9%84%EC%95%84+%EC%86%94%EB%A6%AC%ED%85%8C%EC%96%B4/@-23.5805256,14.9642828,9.05z/data=!4m6!3m5!1s0x1c731a93fc9fae0d:0xc238afe9f76ca6f7!8m2!3d-23.8933454!4d16.0045091!16zL20vMGdidHR2?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>시즈리엠 캠프사이트 - NWR</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -214,10 +206,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>포인트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>https://www.google.com/maps/place/%EC%86%8C%EC%84%9C%EC%8A%A4%EB%B8%94%EB%A0%88%EC%9D%B4/@-24.7299883,15.3195806,17z/data=!3m1!4b1!4m6!3m5!1s0x1c720c36bf4379af:0xc1101aae1ad9c253!8m2!3d-24.7299883!4d15.3221555!16s%2Fg%2F1wf4qtjb?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -282,6 +270,10 @@
   </si>
   <si>
     <t>https://www.google.com/maps/place/%EC%84%B8%EB%A0%8C%EC%A7%80%ED%8B%B0+%EA%B5%AD%EB%A6%BD%EA%B3%B5%EC%9B%90/@-2.3188676,34.8236987,13.14z/data=!4m6!3m5!1s0x1832cdd680dac6d1:0x2ea157f39deb3945!8m2!3d-2.3333333!4d34.8333333!16zL20vMGdrM24?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관광지</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -863,7 +855,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -881,7 +873,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>11</v>
@@ -910,10 +902,10 @@
         <v>12</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -978,10 +970,10 @@
         <v>12</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -995,10 +987,10 @@
         <v>12</v>
       </c>
       <c r="D7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1009,13 +1001,13 @@
         <v>45630</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1043,13 +1035,13 @@
         <v>45631</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1077,13 +1069,13 @@
         <v>45632</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1097,10 +1089,10 @@
         <v>13</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1111,13 +1103,13 @@
         <v>45633</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1131,10 +1123,10 @@
         <v>12</v>
       </c>
       <c r="D15" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1148,10 +1140,10 @@
         <v>12</v>
       </c>
       <c r="D16" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1165,10 +1157,10 @@
         <v>13</v>
       </c>
       <c r="D17" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1182,10 +1174,10 @@
         <v>12</v>
       </c>
       <c r="D18" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1196,13 +1188,13 @@
         <v>45634</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1216,10 +1208,10 @@
         <v>13</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1230,13 +1222,13 @@
         <v>45635</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1247,13 +1239,13 @@
         <v>45635</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1264,13 +1256,13 @@
         <v>45635</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="10" t="s">
-        <v>47</v>
-      </c>
       <c r="E23" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1281,13 +1273,13 @@
         <v>45635</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1298,13 +1290,13 @@
         <v>45635</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="D25" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1315,13 +1307,13 @@
         <v>45635</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1335,10 +1327,10 @@
         <v>13</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1349,13 +1341,13 @@
         <v>45636</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1366,13 +1358,13 @@
         <v>45636</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1386,10 +1378,10 @@
         <v>13</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1403,10 +1395,10 @@
         <v>12</v>
       </c>
       <c r="D31" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1437,10 +1429,10 @@
         <v>12</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1460,23 +1452,23 @@
     <hyperlink ref="E16" r:id="rId12" display="https://www.google.com/maps/place/O.R.+%ED%83%90%EB%B3%B4+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@-26.1393913,28.24422,17z/data=!3m1!4b1!4m6!3m5!1s0x1e95143805a229c3:0xb3bf1c40792821d6!8m2!3d-26.1393913!4d28.2467949!16zL20vMHFuMnY?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{14654894-8722-49A5-8EBE-69B3C3DC3F81}"/>
     <hyperlink ref="E17" r:id="rId13" display="https://www.google.com/maps/place/Peermont+Metcourt+Hotel/@-26.1434586,28.2259394,15.41z/data=!4m9!3m8!1s0x1e9514172b9aaaab:0x6c48ef337d469c96!5m2!4m1!1i2!8m2!3d-26.146848!4d28.2233394!16s%2Fg%2F11c6_xs_nm?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{458D5807-E8BD-4531-81BF-D64E6223E73C}"/>
     <hyperlink ref="E18" r:id="rId14" display="https://www.google.com/maps/place/%ED%98%B8%EC%84%B8%EC%95%84+%EC%BF%A0%ED%83%80%EC%BD%94+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@-22.4870895,17.4605708,17z/data=!3m1!4b1!4m6!3m5!1s0x1c0badf2ca7a7217:0x1f24b8f61198d350!8m2!3d-22.4870895!4d17.4631457!16zL20vMDd6a2Mx?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{50D57E02-CE7D-4086-BDE0-5961FB898C69}"/>
-    <hyperlink ref="E19" r:id="rId15" display="https://www.google.com/maps/place/%EB%82%98%EB%AF%B8%EB%B9%84%EC%95%84+%EC%86%94%EB%A6%AC%ED%85%8C%EC%96%B4/@-23.5805256,14.9642828,9.05z/data=!4m6!3m5!1s0x1c731a93fc9fae0d:0xc238afe9f76ca6f7!8m2!3d-23.8933454!4d16.0045091!16zL20vMGdidHR2?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{A54A5E32-196D-42F9-91C4-365C692861C5}"/>
-    <hyperlink ref="E20" r:id="rId16" display="https://www.google.com/maps/place/%EC%8B%9C%EC%A6%88%EB%A6%AC%EC%97%A0+%EC%BA%A0%ED%94%84%EC%82%AC%EC%9D%B4%ED%8A%B8+-+NWR/@-24.4500775,15.7506268,12z/data=!4m9!3m8!1s0x1c728a898f99a62b:0x2e1eb267fbdbc249!5m2!4m1!1i2!8m2!3d-24.4862708!4d15.7990914!16s%2Fg%2F11cn0qm_4c?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{7B6FC9C3-8F51-42F6-AD33-00DE6263C199}"/>
-    <hyperlink ref="E21" r:id="rId17" xr:uid="{CD9111B8-EA78-457F-93E5-73D21B5D8356}"/>
-    <hyperlink ref="E22" r:id="rId18" display="https://www.google.com/maps/place/%EC%86%8C%EC%84%9C%EC%8A%A4%EB%B8%94%EB%A0%88%EC%9D%B4/@-24.7299883,15.3195806,17z/data=!3m1!4b1!4m6!3m5!1s0x1c720c36bf4379af:0xc1101aae1ad9c253!8m2!3d-24.7299883!4d15.3221555!16s%2Fg%2F1wf4qtjb?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{C9726F3B-461C-4996-B5B1-2045879CD9E6}"/>
-    <hyperlink ref="E23" r:id="rId19" display="https://www.google.com/maps/place/%EB%8D%B0%EB%93%9C%EB%B8%8C%EB%A0%88%EC%9D%B4/@-24.7592732,15.2923894,17z/data=!4m6!3m5!1s0x1c720eb85269ca25:0x91e505d54330767b!8m2!3d-24.7592732!4d15.2923894!16s%2Fm%2F03wbkkh?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{D153F76A-5342-4966-9F4E-7039CAC3EFFB}"/>
-    <hyperlink ref="E24" r:id="rId20" display="https://www.google.com/maps/place/%EC%8B%9C%EC%A6%88%EB%A6%AC%EC%97%A0+%EC%BA%A0%ED%94%84%EC%82%AC%EC%9D%B4%ED%8A%B8+-+NWR/@-24.4500775,15.7506268,12z/data=!4m9!3m8!1s0x1c728a898f99a62b:0x2e1eb267fbdbc249!5m2!4m1!1i2!8m2!3d-24.4862708!4d15.7990914!16s%2Fg%2F11cn0qm_4c?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{BE57540F-46CF-4A8A-BA58-CB578556E112}"/>
-    <hyperlink ref="E26" r:id="rId21" xr:uid="{BF67EE91-A621-4922-8560-9E32325A205B}"/>
-    <hyperlink ref="E25" r:id="rId22" xr:uid="{E16FD79B-BCAC-47DD-B786-5230F7955562}"/>
-    <hyperlink ref="E27" r:id="rId23" display="https://www.google.com/maps/place/%EC%8B%9C%EC%A6%88%EB%A6%AC%EC%97%A0+%EC%BA%A0%ED%94%84%EC%82%AC%EC%9D%B4%ED%8A%B8+-+NWR/@-24.4500775,15.7506268,12z/data=!4m9!3m8!1s0x1c728a898f99a62b:0x2e1eb267fbdbc249!5m2!4m1!1i2!8m2!3d-24.4862708!4d15.7990914!16s%2Fg%2F11cn0qm_4c?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{8E02571A-AD76-4D04-AEAE-91F8982B7CCA}"/>
-    <hyperlink ref="E28" r:id="rId24" xr:uid="{FF0AF7DC-497E-419B-9F68-CE34EC44E922}"/>
-    <hyperlink ref="E29" r:id="rId25" display="https://www.google.com/maps/place/%EB%82%98%EB%AF%B8%EB%B9%84%EC%95%84+%EB%B9%88%ED%8A%B8%ED%9B%84%ED%81%AC/@-22.563751,17.0210266,13z/data=!3m1!4b1!4m6!3m5!1s0x1c0b1b5cb30c01ed:0xe4b84940cc445d3b!8m2!3d-22.5649344!4d17.0842147!16zL20vMGZ0cTc?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{D10D4065-5F67-4E23-8B6E-5C4E78C39A3B}"/>
-    <hyperlink ref="E30" r:id="rId26" display="https://www.google.com/maps/place/Hilton+Garden+Inn+Windhoek/@-22.569885,17.0830968,17z/data=!3m1!4b1!4m9!3m8!1s0x1c0b1b6b8586b239:0xf1a0bbc930def090!5m2!4m1!1i2!8m2!3d-22.569885!4d17.0856717!16s%2Fg%2F11vwm83dz3?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{00A71145-DBE9-438B-8868-7790C10802F8}"/>
-    <hyperlink ref="E31" r:id="rId27" display="https://www.google.com/maps/place/%ED%98%B8%EC%84%B8%EC%95%84+%EC%BF%A0%ED%83%80%EC%BD%94+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@-22.4870895,17.4605708,17z/data=!3m1!4b1!4m6!3m5!1s0x1c0badf2ca7a7217:0x1f24b8f61198d350!8m2!3d-22.4870895!4d17.4631457!16zL20vMDd6a2Mx?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{29F1DAEA-277E-466A-A40C-3FFE02FFD2AF}"/>
-    <hyperlink ref="E32" r:id="rId28" display="https://www.google.com/maps/place/%EC%95%84%EB%94%94%EC%8A%A4%EC%95%84%EB%B0%94%EB%B0%94+%EB%B3%BC%EB%A0%88+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@8.9837932,38.7937261,17z/data=!3m1!4b1!4m6!3m5!1s0x164b858fbf50bd97:0x93a0799b20ab0276!8m2!3d8.9837879!4d38.7963064!16zL20vMDQ3OTc4?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{E4AA03EF-7BBE-460D-8949-AF4516B7AB09}"/>
-    <hyperlink ref="E33" r:id="rId29" display="https://www.google.com/maps/place/%EC%9D%B8%EC%B2%9C%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/data=!3m1!4b1!4m6!3m5!1s0x357b9a833a5efa59:0x8d4ba096cb5cbed4!8m2!3d37.458666!4d126.4419679!16zL20vMDE2MWdi?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{3D8D0619-FED2-4E3C-A6EE-A3EED824D44A}"/>
-    <hyperlink ref="E8" r:id="rId30" display="https://www.google.com/maps/place/%EC%84%B8%EB%A0%8C%EC%A7%80%ED%8B%B0+%EA%B5%AD%EB%A6%BD%EA%B3%B5%EC%9B%90/@-2.3188676,34.8236987,13.14z/data=!4m6!3m5!1s0x1832cdd680dac6d1:0x2ea157f39deb3945!8m2!3d-2.3333333!4d34.8333333!16zL20vMGdrM24?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{542A8617-DF23-4039-A526-CCCE0B9271A2}"/>
-    <hyperlink ref="E10" r:id="rId31" display="https://www.google.com/maps/place/%EC%84%B8%EB%A0%8C%EC%A7%80%ED%8B%B0+%EA%B5%AD%EB%A6%BD%EA%B3%B5%EC%9B%90/@-2.3188676,34.8236987,13.14z/data=!4m6!3m5!1s0x1832cdd680dac6d1:0x2ea157f39deb3945!8m2!3d-2.3333333!4d34.8333333!16zL20vMGdrM24?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{D23A16AE-A251-41CF-B1FC-19D241B22301}"/>
+    <hyperlink ref="E20" r:id="rId15" display="https://www.google.com/maps/place/%EC%8B%9C%EC%A6%88%EB%A6%AC%EC%97%A0+%EC%BA%A0%ED%94%84%EC%82%AC%EC%9D%B4%ED%8A%B8+-+NWR/@-24.4500775,15.7506268,12z/data=!4m9!3m8!1s0x1c728a898f99a62b:0x2e1eb267fbdbc249!5m2!4m1!1i2!8m2!3d-24.4862708!4d15.7990914!16s%2Fg%2F11cn0qm_4c?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{7B6FC9C3-8F51-42F6-AD33-00DE6263C199}"/>
+    <hyperlink ref="E21" r:id="rId16" xr:uid="{CD9111B8-EA78-457F-93E5-73D21B5D8356}"/>
+    <hyperlink ref="E22" r:id="rId17" display="https://www.google.com/maps/place/%EC%86%8C%EC%84%9C%EC%8A%A4%EB%B8%94%EB%A0%88%EC%9D%B4/@-24.7299883,15.3195806,17z/data=!3m1!4b1!4m6!3m5!1s0x1c720c36bf4379af:0xc1101aae1ad9c253!8m2!3d-24.7299883!4d15.3221555!16s%2Fg%2F1wf4qtjb?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{C9726F3B-461C-4996-B5B1-2045879CD9E6}"/>
+    <hyperlink ref="E23" r:id="rId18" display="https://www.google.com/maps/place/%EB%8D%B0%EB%93%9C%EB%B8%8C%EB%A0%88%EC%9D%B4/@-24.7592732,15.2923894,17z/data=!4m6!3m5!1s0x1c720eb85269ca25:0x91e505d54330767b!8m2!3d-24.7592732!4d15.2923894!16s%2Fm%2F03wbkkh?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{D153F76A-5342-4966-9F4E-7039CAC3EFFB}"/>
+    <hyperlink ref="E24" r:id="rId19" display="https://www.google.com/maps/place/%EC%8B%9C%EC%A6%88%EB%A6%AC%EC%97%A0+%EC%BA%A0%ED%94%84%EC%82%AC%EC%9D%B4%ED%8A%B8+-+NWR/@-24.4500775,15.7506268,12z/data=!4m9!3m8!1s0x1c728a898f99a62b:0x2e1eb267fbdbc249!5m2!4m1!1i2!8m2!3d-24.4862708!4d15.7990914!16s%2Fg%2F11cn0qm_4c?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{BE57540F-46CF-4A8A-BA58-CB578556E112}"/>
+    <hyperlink ref="E26" r:id="rId20" xr:uid="{BF67EE91-A621-4922-8560-9E32325A205B}"/>
+    <hyperlink ref="E25" r:id="rId21" xr:uid="{E16FD79B-BCAC-47DD-B786-5230F7955562}"/>
+    <hyperlink ref="E27" r:id="rId22" display="https://www.google.com/maps/place/%EC%8B%9C%EC%A6%88%EB%A6%AC%EC%97%A0+%EC%BA%A0%ED%94%84%EC%82%AC%EC%9D%B4%ED%8A%B8+-+NWR/@-24.4500775,15.7506268,12z/data=!4m9!3m8!1s0x1c728a898f99a62b:0x2e1eb267fbdbc249!5m2!4m1!1i2!8m2!3d-24.4862708!4d15.7990914!16s%2Fg%2F11cn0qm_4c?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{8E02571A-AD76-4D04-AEAE-91F8982B7CCA}"/>
+    <hyperlink ref="E28" r:id="rId23" xr:uid="{FF0AF7DC-497E-419B-9F68-CE34EC44E922}"/>
+    <hyperlink ref="E29" r:id="rId24" display="https://www.google.com/maps/place/%EB%82%98%EB%AF%B8%EB%B9%84%EC%95%84+%EB%B9%88%ED%8A%B8%ED%9B%84%ED%81%AC/@-22.563751,17.0210266,13z/data=!3m1!4b1!4m6!3m5!1s0x1c0b1b5cb30c01ed:0xe4b84940cc445d3b!8m2!3d-22.5649344!4d17.0842147!16zL20vMGZ0cTc?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{D10D4065-5F67-4E23-8B6E-5C4E78C39A3B}"/>
+    <hyperlink ref="E30" r:id="rId25" display="https://www.google.com/maps/place/Hilton+Garden+Inn+Windhoek/@-22.569885,17.0830968,17z/data=!3m1!4b1!4m9!3m8!1s0x1c0b1b6b8586b239:0xf1a0bbc930def090!5m2!4m1!1i2!8m2!3d-22.569885!4d17.0856717!16s%2Fg%2F11vwm83dz3?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{00A71145-DBE9-438B-8868-7790C10802F8}"/>
+    <hyperlink ref="E31" r:id="rId26" display="https://www.google.com/maps/place/%ED%98%B8%EC%84%B8%EC%95%84+%EC%BF%A0%ED%83%80%EC%BD%94+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@-22.4870895,17.4605708,17z/data=!3m1!4b1!4m6!3m5!1s0x1c0badf2ca7a7217:0x1f24b8f61198d350!8m2!3d-22.4870895!4d17.4631457!16zL20vMDd6a2Mx?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{29F1DAEA-277E-466A-A40C-3FFE02FFD2AF}"/>
+    <hyperlink ref="E32" r:id="rId27" display="https://www.google.com/maps/place/%EC%95%84%EB%94%94%EC%8A%A4%EC%95%84%EB%B0%94%EB%B0%94+%EB%B3%BC%EB%A0%88+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@8.9837932,38.7937261,17z/data=!3m1!4b1!4m6!3m5!1s0x164b858fbf50bd97:0x93a0799b20ab0276!8m2!3d8.9837879!4d38.7963064!16zL20vMDQ3OTc4?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{E4AA03EF-7BBE-460D-8949-AF4516B7AB09}"/>
+    <hyperlink ref="E33" r:id="rId28" display="https://www.google.com/maps/place/%EC%9D%B8%EC%B2%9C%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/data=!3m1!4b1!4m6!3m5!1s0x357b9a833a5efa59:0x8d4ba096cb5cbed4!8m2!3d37.458666!4d126.4419679!16zL20vMDE2MWdi?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{3D8D0619-FED2-4E3C-A6EE-A3EED824D44A}"/>
+    <hyperlink ref="E8" r:id="rId29" display="https://www.google.com/maps/place/%EC%84%B8%EB%A0%8C%EC%A7%80%ED%8B%B0+%EA%B5%AD%EB%A6%BD%EA%B3%B5%EC%9B%90/@-2.3188676,34.8236987,13.14z/data=!4m6!3m5!1s0x1832cdd680dac6d1:0x2ea157f39deb3945!8m2!3d-2.3333333!4d34.8333333!16zL20vMGdrM24?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{542A8617-DF23-4039-A526-CCCE0B9271A2}"/>
+    <hyperlink ref="E10" r:id="rId30" display="https://www.google.com/maps/place/%EC%84%B8%EB%A0%8C%EC%A7%80%ED%8B%B0+%EA%B5%AD%EB%A6%BD%EA%B3%B5%EC%9B%90/@-2.3188676,34.8236987,13.14z/data=!4m6!3m5!1s0x1832cdd680dac6d1:0x2ea157f39deb3945!8m2!3d-2.3333333!4d34.8333333!16zL20vMGdrM24?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{D23A16AE-A251-41CF-B1FC-19D241B22301}"/>
+    <hyperlink ref="E19" r:id="rId31" xr:uid="{CCB97CBB-F83B-4F4D-8651-7EDD4F5D2BAB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>

</xml_diff>

<commit_message>
No13: 아루샤 -> Arusha airport
</commit_message>
<xml_diff>
--- a/Honeymoon_Locations.xlsx
+++ b/Honeymoon_Locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HJ\Python\HoneyMoon_Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6337605C-C67B-4BA0-A12B-B487C5207A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9EB443-B6FA-4CB5-8D96-F1370C24A5F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{5554A70D-75DD-49DE-8066-5822D9CA01A4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
   <si>
     <t>위도</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -143,14 +143,6 @@
   </si>
   <si>
     <t>경유</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/%ED%83%84%EC%9E%90%EB%8B%88%EC%95%84+%EC%95%84%EB%A3%A8%EC%83%A4/@-3.38176,36.7018778,11.64z/data=!4m6!3m5!1s0x18371c88f2387383:0xbc1907f7ec497152!8m2!3d-3.3869254!4d36.6829927!16zL20vMDFfZnB4?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아루샤</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -855,7 +847,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="N39" sqref="M39:N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -902,10 +894,10 @@
         <v>12</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1001,13 +993,13 @@
         <v>45630</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1035,13 +1027,13 @@
         <v>45631</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1069,7 +1061,7 @@
         <v>45632</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>16</v>
@@ -1103,13 +1095,13 @@
         <v>45633</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1123,10 +1115,10 @@
         <v>12</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1140,10 +1132,10 @@
         <v>12</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1157,10 +1149,10 @@
         <v>13</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1174,10 +1166,10 @@
         <v>12</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1191,10 +1183,10 @@
         <v>26</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1208,10 +1200,10 @@
         <v>13</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1222,13 +1214,13 @@
         <v>45635</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1239,13 +1231,13 @@
         <v>45635</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1256,13 +1248,13 @@
         <v>45635</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1276,10 +1268,10 @@
         <v>26</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1290,13 +1282,13 @@
         <v>45635</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1307,13 +1299,13 @@
         <v>45635</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1327,10 +1319,10 @@
         <v>13</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1344,10 +1336,10 @@
         <v>26</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1361,10 +1353,10 @@
         <v>26</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1378,10 +1370,10 @@
         <v>13</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1395,10 +1387,10 @@
         <v>12</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1429,10 +1421,10 @@
         <v>12</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1447,28 +1439,28 @@
     <hyperlink ref="E7" r:id="rId7" xr:uid="{64BD1B95-6F2C-4FBC-AF81-824A5877CD58}"/>
     <hyperlink ref="E13" r:id="rId8" xr:uid="{43CB55A1-C847-44CE-92C4-089D4CC36279}"/>
     <hyperlink ref="E6" r:id="rId9" xr:uid="{659B9DCA-168A-4400-82AB-E4206FE6ED1D}"/>
-    <hyperlink ref="E14" r:id="rId10" display="https://www.google.com/maps/place/%ED%83%84%EC%9E%90%EB%8B%88%EC%95%84+%EC%95%84%EB%A3%A8%EC%83%A4/@-3.38176,36.7018778,11.64z/data=!4m6!3m5!1s0x18371c88f2387383:0xbc1907f7ec497152!8m2!3d-3.3869254!4d36.6829927!16zL20vMDFfZnB4?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{70F5439D-DB4A-490E-8117-AD29F46EFF02}"/>
-    <hyperlink ref="E15" r:id="rId11" display="https://www.google.com/maps/place/%EC%A1%B0%EB%AA%A8+%EC%BC%80%EB%83%90%ED%83%80+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@-1.3225242,36.9219546,17z/data=!3m1!4b1!4m6!3m5!1s0x182f129102505cef:0xefc58e7ef0660bf2!8m2!3d-1.3225242!4d36.9245295!16zL20vMDExemNy?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{387A00FE-565F-4D9E-B858-DE60D80E138F}"/>
-    <hyperlink ref="E16" r:id="rId12" display="https://www.google.com/maps/place/O.R.+%ED%83%90%EB%B3%B4+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@-26.1393913,28.24422,17z/data=!3m1!4b1!4m6!3m5!1s0x1e95143805a229c3:0xb3bf1c40792821d6!8m2!3d-26.1393913!4d28.2467949!16zL20vMHFuMnY?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{14654894-8722-49A5-8EBE-69B3C3DC3F81}"/>
-    <hyperlink ref="E17" r:id="rId13" display="https://www.google.com/maps/place/Peermont+Metcourt+Hotel/@-26.1434586,28.2259394,15.41z/data=!4m9!3m8!1s0x1e9514172b9aaaab:0x6c48ef337d469c96!5m2!4m1!1i2!8m2!3d-26.146848!4d28.2233394!16s%2Fg%2F11c6_xs_nm?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{458D5807-E8BD-4531-81BF-D64E6223E73C}"/>
-    <hyperlink ref="E18" r:id="rId14" display="https://www.google.com/maps/place/%ED%98%B8%EC%84%B8%EC%95%84+%EC%BF%A0%ED%83%80%EC%BD%94+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@-22.4870895,17.4605708,17z/data=!3m1!4b1!4m6!3m5!1s0x1c0badf2ca7a7217:0x1f24b8f61198d350!8m2!3d-22.4870895!4d17.4631457!16zL20vMDd6a2Mx?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{50D57E02-CE7D-4086-BDE0-5961FB898C69}"/>
-    <hyperlink ref="E20" r:id="rId15" display="https://www.google.com/maps/place/%EC%8B%9C%EC%A6%88%EB%A6%AC%EC%97%A0+%EC%BA%A0%ED%94%84%EC%82%AC%EC%9D%B4%ED%8A%B8+-+NWR/@-24.4500775,15.7506268,12z/data=!4m9!3m8!1s0x1c728a898f99a62b:0x2e1eb267fbdbc249!5m2!4m1!1i2!8m2!3d-24.4862708!4d15.7990914!16s%2Fg%2F11cn0qm_4c?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{7B6FC9C3-8F51-42F6-AD33-00DE6263C199}"/>
-    <hyperlink ref="E21" r:id="rId16" xr:uid="{CD9111B8-EA78-457F-93E5-73D21B5D8356}"/>
-    <hyperlink ref="E22" r:id="rId17" display="https://www.google.com/maps/place/%EC%86%8C%EC%84%9C%EC%8A%A4%EB%B8%94%EB%A0%88%EC%9D%B4/@-24.7299883,15.3195806,17z/data=!3m1!4b1!4m6!3m5!1s0x1c720c36bf4379af:0xc1101aae1ad9c253!8m2!3d-24.7299883!4d15.3221555!16s%2Fg%2F1wf4qtjb?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{C9726F3B-461C-4996-B5B1-2045879CD9E6}"/>
-    <hyperlink ref="E23" r:id="rId18" display="https://www.google.com/maps/place/%EB%8D%B0%EB%93%9C%EB%B8%8C%EB%A0%88%EC%9D%B4/@-24.7592732,15.2923894,17z/data=!4m6!3m5!1s0x1c720eb85269ca25:0x91e505d54330767b!8m2!3d-24.7592732!4d15.2923894!16s%2Fm%2F03wbkkh?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{D153F76A-5342-4966-9F4E-7039CAC3EFFB}"/>
-    <hyperlink ref="E24" r:id="rId19" display="https://www.google.com/maps/place/%EC%8B%9C%EC%A6%88%EB%A6%AC%EC%97%A0+%EC%BA%A0%ED%94%84%EC%82%AC%EC%9D%B4%ED%8A%B8+-+NWR/@-24.4500775,15.7506268,12z/data=!4m9!3m8!1s0x1c728a898f99a62b:0x2e1eb267fbdbc249!5m2!4m1!1i2!8m2!3d-24.4862708!4d15.7990914!16s%2Fg%2F11cn0qm_4c?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{BE57540F-46CF-4A8A-BA58-CB578556E112}"/>
-    <hyperlink ref="E26" r:id="rId20" xr:uid="{BF67EE91-A621-4922-8560-9E32325A205B}"/>
-    <hyperlink ref="E25" r:id="rId21" xr:uid="{E16FD79B-BCAC-47DD-B786-5230F7955562}"/>
-    <hyperlink ref="E27" r:id="rId22" display="https://www.google.com/maps/place/%EC%8B%9C%EC%A6%88%EB%A6%AC%EC%97%A0+%EC%BA%A0%ED%94%84%EC%82%AC%EC%9D%B4%ED%8A%B8+-+NWR/@-24.4500775,15.7506268,12z/data=!4m9!3m8!1s0x1c728a898f99a62b:0x2e1eb267fbdbc249!5m2!4m1!1i2!8m2!3d-24.4862708!4d15.7990914!16s%2Fg%2F11cn0qm_4c?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{8E02571A-AD76-4D04-AEAE-91F8982B7CCA}"/>
-    <hyperlink ref="E28" r:id="rId23" xr:uid="{FF0AF7DC-497E-419B-9F68-CE34EC44E922}"/>
-    <hyperlink ref="E29" r:id="rId24" display="https://www.google.com/maps/place/%EB%82%98%EB%AF%B8%EB%B9%84%EC%95%84+%EB%B9%88%ED%8A%B8%ED%9B%84%ED%81%AC/@-22.563751,17.0210266,13z/data=!3m1!4b1!4m6!3m5!1s0x1c0b1b5cb30c01ed:0xe4b84940cc445d3b!8m2!3d-22.5649344!4d17.0842147!16zL20vMGZ0cTc?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{D10D4065-5F67-4E23-8B6E-5C4E78C39A3B}"/>
-    <hyperlink ref="E30" r:id="rId25" display="https://www.google.com/maps/place/Hilton+Garden+Inn+Windhoek/@-22.569885,17.0830968,17z/data=!3m1!4b1!4m9!3m8!1s0x1c0b1b6b8586b239:0xf1a0bbc930def090!5m2!4m1!1i2!8m2!3d-22.569885!4d17.0856717!16s%2Fg%2F11vwm83dz3?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{00A71145-DBE9-438B-8868-7790C10802F8}"/>
-    <hyperlink ref="E31" r:id="rId26" display="https://www.google.com/maps/place/%ED%98%B8%EC%84%B8%EC%95%84+%EC%BF%A0%ED%83%80%EC%BD%94+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@-22.4870895,17.4605708,17z/data=!3m1!4b1!4m6!3m5!1s0x1c0badf2ca7a7217:0x1f24b8f61198d350!8m2!3d-22.4870895!4d17.4631457!16zL20vMDd6a2Mx?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{29F1DAEA-277E-466A-A40C-3FFE02FFD2AF}"/>
-    <hyperlink ref="E32" r:id="rId27" display="https://www.google.com/maps/place/%EC%95%84%EB%94%94%EC%8A%A4%EC%95%84%EB%B0%94%EB%B0%94+%EB%B3%BC%EB%A0%88+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@8.9837932,38.7937261,17z/data=!3m1!4b1!4m6!3m5!1s0x164b858fbf50bd97:0x93a0799b20ab0276!8m2!3d8.9837879!4d38.7963064!16zL20vMDQ3OTc4?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{E4AA03EF-7BBE-460D-8949-AF4516B7AB09}"/>
-    <hyperlink ref="E33" r:id="rId28" display="https://www.google.com/maps/place/%EC%9D%B8%EC%B2%9C%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/data=!3m1!4b1!4m6!3m5!1s0x357b9a833a5efa59:0x8d4ba096cb5cbed4!8m2!3d37.458666!4d126.4419679!16zL20vMDE2MWdi?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{3D8D0619-FED2-4E3C-A6EE-A3EED824D44A}"/>
-    <hyperlink ref="E8" r:id="rId29" display="https://www.google.com/maps/place/%EC%84%B8%EB%A0%8C%EC%A7%80%ED%8B%B0+%EA%B5%AD%EB%A6%BD%EA%B3%B5%EC%9B%90/@-2.3188676,34.8236987,13.14z/data=!4m6!3m5!1s0x1832cdd680dac6d1:0x2ea157f39deb3945!8m2!3d-2.3333333!4d34.8333333!16zL20vMGdrM24?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{542A8617-DF23-4039-A526-CCCE0B9271A2}"/>
-    <hyperlink ref="E10" r:id="rId30" display="https://www.google.com/maps/place/%EC%84%B8%EB%A0%8C%EC%A7%80%ED%8B%B0+%EA%B5%AD%EB%A6%BD%EA%B3%B5%EC%9B%90/@-2.3188676,34.8236987,13.14z/data=!4m6!3m5!1s0x1832cdd680dac6d1:0x2ea157f39deb3945!8m2!3d-2.3333333!4d34.8333333!16zL20vMGdrM24?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{D23A16AE-A251-41CF-B1FC-19D241B22301}"/>
-    <hyperlink ref="E19" r:id="rId31" xr:uid="{CCB97CBB-F83B-4F4D-8651-7EDD4F5D2BAB}"/>
+    <hyperlink ref="E15" r:id="rId10" display="https://www.google.com/maps/place/%EC%A1%B0%EB%AA%A8+%EC%BC%80%EB%83%90%ED%83%80+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@-1.3225242,36.9219546,17z/data=!3m1!4b1!4m6!3m5!1s0x182f129102505cef:0xefc58e7ef0660bf2!8m2!3d-1.3225242!4d36.9245295!16zL20vMDExemNy?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{387A00FE-565F-4D9E-B858-DE60D80E138F}"/>
+    <hyperlink ref="E16" r:id="rId11" display="https://www.google.com/maps/place/O.R.+%ED%83%90%EB%B3%B4+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@-26.1393913,28.24422,17z/data=!3m1!4b1!4m6!3m5!1s0x1e95143805a229c3:0xb3bf1c40792821d6!8m2!3d-26.1393913!4d28.2467949!16zL20vMHFuMnY?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{14654894-8722-49A5-8EBE-69B3C3DC3F81}"/>
+    <hyperlink ref="E17" r:id="rId12" display="https://www.google.com/maps/place/Peermont+Metcourt+Hotel/@-26.1434586,28.2259394,15.41z/data=!4m9!3m8!1s0x1e9514172b9aaaab:0x6c48ef337d469c96!5m2!4m1!1i2!8m2!3d-26.146848!4d28.2233394!16s%2Fg%2F11c6_xs_nm?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{458D5807-E8BD-4531-81BF-D64E6223E73C}"/>
+    <hyperlink ref="E18" r:id="rId13" display="https://www.google.com/maps/place/%ED%98%B8%EC%84%B8%EC%95%84+%EC%BF%A0%ED%83%80%EC%BD%94+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@-22.4870895,17.4605708,17z/data=!3m1!4b1!4m6!3m5!1s0x1c0badf2ca7a7217:0x1f24b8f61198d350!8m2!3d-22.4870895!4d17.4631457!16zL20vMDd6a2Mx?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{50D57E02-CE7D-4086-BDE0-5961FB898C69}"/>
+    <hyperlink ref="E20" r:id="rId14" display="https://www.google.com/maps/place/%EC%8B%9C%EC%A6%88%EB%A6%AC%EC%97%A0+%EC%BA%A0%ED%94%84%EC%82%AC%EC%9D%B4%ED%8A%B8+-+NWR/@-24.4500775,15.7506268,12z/data=!4m9!3m8!1s0x1c728a898f99a62b:0x2e1eb267fbdbc249!5m2!4m1!1i2!8m2!3d-24.4862708!4d15.7990914!16s%2Fg%2F11cn0qm_4c?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{7B6FC9C3-8F51-42F6-AD33-00DE6263C199}"/>
+    <hyperlink ref="E21" r:id="rId15" xr:uid="{CD9111B8-EA78-457F-93E5-73D21B5D8356}"/>
+    <hyperlink ref="E22" r:id="rId16" display="https://www.google.com/maps/place/%EC%86%8C%EC%84%9C%EC%8A%A4%EB%B8%94%EB%A0%88%EC%9D%B4/@-24.7299883,15.3195806,17z/data=!3m1!4b1!4m6!3m5!1s0x1c720c36bf4379af:0xc1101aae1ad9c253!8m2!3d-24.7299883!4d15.3221555!16s%2Fg%2F1wf4qtjb?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{C9726F3B-461C-4996-B5B1-2045879CD9E6}"/>
+    <hyperlink ref="E23" r:id="rId17" display="https://www.google.com/maps/place/%EB%8D%B0%EB%93%9C%EB%B8%8C%EB%A0%88%EC%9D%B4/@-24.7592732,15.2923894,17z/data=!4m6!3m5!1s0x1c720eb85269ca25:0x91e505d54330767b!8m2!3d-24.7592732!4d15.2923894!16s%2Fm%2F03wbkkh?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{D153F76A-5342-4966-9F4E-7039CAC3EFFB}"/>
+    <hyperlink ref="E24" r:id="rId18" display="https://www.google.com/maps/place/%EC%8B%9C%EC%A6%88%EB%A6%AC%EC%97%A0+%EC%BA%A0%ED%94%84%EC%82%AC%EC%9D%B4%ED%8A%B8+-+NWR/@-24.4500775,15.7506268,12z/data=!4m9!3m8!1s0x1c728a898f99a62b:0x2e1eb267fbdbc249!5m2!4m1!1i2!8m2!3d-24.4862708!4d15.7990914!16s%2Fg%2F11cn0qm_4c?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{BE57540F-46CF-4A8A-BA58-CB578556E112}"/>
+    <hyperlink ref="E26" r:id="rId19" xr:uid="{BF67EE91-A621-4922-8560-9E32325A205B}"/>
+    <hyperlink ref="E25" r:id="rId20" xr:uid="{E16FD79B-BCAC-47DD-B786-5230F7955562}"/>
+    <hyperlink ref="E27" r:id="rId21" display="https://www.google.com/maps/place/%EC%8B%9C%EC%A6%88%EB%A6%AC%EC%97%A0+%EC%BA%A0%ED%94%84%EC%82%AC%EC%9D%B4%ED%8A%B8+-+NWR/@-24.4500775,15.7506268,12z/data=!4m9!3m8!1s0x1c728a898f99a62b:0x2e1eb267fbdbc249!5m2!4m1!1i2!8m2!3d-24.4862708!4d15.7990914!16s%2Fg%2F11cn0qm_4c?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{8E02571A-AD76-4D04-AEAE-91F8982B7CCA}"/>
+    <hyperlink ref="E28" r:id="rId22" xr:uid="{FF0AF7DC-497E-419B-9F68-CE34EC44E922}"/>
+    <hyperlink ref="E29" r:id="rId23" display="https://www.google.com/maps/place/%EB%82%98%EB%AF%B8%EB%B9%84%EC%95%84+%EB%B9%88%ED%8A%B8%ED%9B%84%ED%81%AC/@-22.563751,17.0210266,13z/data=!3m1!4b1!4m6!3m5!1s0x1c0b1b5cb30c01ed:0xe4b84940cc445d3b!8m2!3d-22.5649344!4d17.0842147!16zL20vMGZ0cTc?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{D10D4065-5F67-4E23-8B6E-5C4E78C39A3B}"/>
+    <hyperlink ref="E30" r:id="rId24" display="https://www.google.com/maps/place/Hilton+Garden+Inn+Windhoek/@-22.569885,17.0830968,17z/data=!3m1!4b1!4m9!3m8!1s0x1c0b1b6b8586b239:0xf1a0bbc930def090!5m2!4m1!1i2!8m2!3d-22.569885!4d17.0856717!16s%2Fg%2F11vwm83dz3?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{00A71145-DBE9-438B-8868-7790C10802F8}"/>
+    <hyperlink ref="E31" r:id="rId25" display="https://www.google.com/maps/place/%ED%98%B8%EC%84%B8%EC%95%84+%EC%BF%A0%ED%83%80%EC%BD%94+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@-22.4870895,17.4605708,17z/data=!3m1!4b1!4m6!3m5!1s0x1c0badf2ca7a7217:0x1f24b8f61198d350!8m2!3d-22.4870895!4d17.4631457!16zL20vMDd6a2Mx?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{29F1DAEA-277E-466A-A40C-3FFE02FFD2AF}"/>
+    <hyperlink ref="E32" r:id="rId26" display="https://www.google.com/maps/place/%EC%95%84%EB%94%94%EC%8A%A4%EC%95%84%EB%B0%94%EB%B0%94+%EB%B3%BC%EB%A0%88+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@8.9837932,38.7937261,17z/data=!3m1!4b1!4m6!3m5!1s0x164b858fbf50bd97:0x93a0799b20ab0276!8m2!3d8.9837879!4d38.7963064!16zL20vMDQ3OTc4?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{E4AA03EF-7BBE-460D-8949-AF4516B7AB09}"/>
+    <hyperlink ref="E33" r:id="rId27" display="https://www.google.com/maps/place/%EC%9D%B8%EC%B2%9C%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/data=!3m1!4b1!4m6!3m5!1s0x357b9a833a5efa59:0x8d4ba096cb5cbed4!8m2!3d37.458666!4d126.4419679!16zL20vMDE2MWdi?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{3D8D0619-FED2-4E3C-A6EE-A3EED824D44A}"/>
+    <hyperlink ref="E8" r:id="rId28" display="https://www.google.com/maps/place/%EC%84%B8%EB%A0%8C%EC%A7%80%ED%8B%B0+%EA%B5%AD%EB%A6%BD%EA%B3%B5%EC%9B%90/@-2.3188676,34.8236987,13.14z/data=!4m6!3m5!1s0x1832cdd680dac6d1:0x2ea157f39deb3945!8m2!3d-2.3333333!4d34.8333333!16zL20vMGdrM24?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{542A8617-DF23-4039-A526-CCCE0B9271A2}"/>
+    <hyperlink ref="E10" r:id="rId29" display="https://www.google.com/maps/place/%EC%84%B8%EB%A0%8C%EC%A7%80%ED%8B%B0+%EA%B5%AD%EB%A6%BD%EA%B3%B5%EC%9B%90/@-2.3188676,34.8236987,13.14z/data=!4m6!3m5!1s0x1832cdd680dac6d1:0x2ea157f39deb3945!8m2!3d-2.3333333!4d34.8333333!16zL20vMGdrM24?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{D23A16AE-A251-41CF-B1FC-19D241B22301}"/>
+    <hyperlink ref="E19" r:id="rId30" xr:uid="{CCB97CBB-F83B-4F4D-8651-7EDD4F5D2BAB}"/>
+    <hyperlink ref="E14" r:id="rId31" xr:uid="{0CFAEB2A-9083-469C-ABAD-67395742ABB3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>

</xml_diff>

<commit_message>
No. 17 (Inserted): O. R. Tambo Intl Airport
</commit_message>
<xml_diff>
--- a/Honeymoon_Locations.xlsx
+++ b/Honeymoon_Locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HJ\Python\HoneyMoon_Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9EB443-B6FA-4CB5-8D96-F1370C24A5F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D0A796-0BAD-455A-9647-FA47214BB8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{5554A70D-75DD-49DE-8066-5822D9CA01A4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
   <si>
     <t>위도</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -844,10 +844,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4573F5-9E6C-4E8C-8DB0-812EE7D0315C}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N39" sqref="M39:N39"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1160,16 +1160,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="9">
-        <v>45634</v>
+        <v>45633</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1180,47 +1180,47 @@
         <v>45634</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="8">
+        <v>19</v>
+      </c>
+      <c r="B20" s="9">
+        <v>45634</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D20" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="11">
-        <v>19</v>
-      </c>
-      <c r="B20" s="6">
+    <row r="21" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="11">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6">
         <v>45634</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C21" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D21" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E21" s="7" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="8">
-        <v>20</v>
-      </c>
-      <c r="B21" s="9">
-        <v>45635</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1234,10 +1234,10 @@
         <v>57</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1251,10 +1251,10 @@
         <v>57</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1265,13 +1265,13 @@
         <v>45635</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1282,13 +1282,13 @@
         <v>45635</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1302,44 +1302,44 @@
         <v>57</v>
       </c>
       <c r="D26" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="8">
+        <v>26</v>
+      </c>
+      <c r="B27" s="9">
+        <v>45635</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="11">
-        <v>26</v>
-      </c>
-      <c r="B27" s="6">
+    <row r="28" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="11">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6">
         <v>45635</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D28" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E28" s="7" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="8">
-        <v>27</v>
-      </c>
-      <c r="B28" s="9">
-        <v>45636</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1353,44 +1353,44 @@
         <v>26</v>
       </c>
       <c r="D29" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="8">
+        <v>29</v>
+      </c>
+      <c r="B30" s="9">
+        <v>45636</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="11">
-        <v>29</v>
-      </c>
-      <c r="B30" s="6">
+    <row r="31" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="11">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6">
         <v>45636</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C31" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D31" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E31" s="7" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="8">
-        <v>30</v>
-      </c>
-      <c r="B31" s="9">
-        <v>45637</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1404,26 +1404,43 @@
         <v>12</v>
       </c>
       <c r="D32" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="8">
+        <v>32</v>
+      </c>
+      <c r="B33" s="9">
+        <v>45637</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="13">
-        <v>32</v>
-      </c>
-      <c r="B33" s="14">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="13">
+        <v>33</v>
+      </c>
+      <c r="B34" s="14">
         <v>45638</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C34" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D34" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1442,27 +1459,28 @@
     <hyperlink ref="E15" r:id="rId10" display="https://www.google.com/maps/place/%EC%A1%B0%EB%AA%A8+%EC%BC%80%EB%83%90%ED%83%80+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@-1.3225242,36.9219546,17z/data=!3m1!4b1!4m6!3m5!1s0x182f129102505cef:0xefc58e7ef0660bf2!8m2!3d-1.3225242!4d36.9245295!16zL20vMDExemNy?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{387A00FE-565F-4D9E-B858-DE60D80E138F}"/>
     <hyperlink ref="E16" r:id="rId11" display="https://www.google.com/maps/place/O.R.+%ED%83%90%EB%B3%B4+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@-26.1393913,28.24422,17z/data=!3m1!4b1!4m6!3m5!1s0x1e95143805a229c3:0xb3bf1c40792821d6!8m2!3d-26.1393913!4d28.2467949!16zL20vMHFuMnY?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{14654894-8722-49A5-8EBE-69B3C3DC3F81}"/>
     <hyperlink ref="E17" r:id="rId12" display="https://www.google.com/maps/place/Peermont+Metcourt+Hotel/@-26.1434586,28.2259394,15.41z/data=!4m9!3m8!1s0x1e9514172b9aaaab:0x6c48ef337d469c96!5m2!4m1!1i2!8m2!3d-26.146848!4d28.2233394!16s%2Fg%2F11c6_xs_nm?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{458D5807-E8BD-4531-81BF-D64E6223E73C}"/>
-    <hyperlink ref="E18" r:id="rId13" display="https://www.google.com/maps/place/%ED%98%B8%EC%84%B8%EC%95%84+%EC%BF%A0%ED%83%80%EC%BD%94+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@-22.4870895,17.4605708,17z/data=!3m1!4b1!4m6!3m5!1s0x1c0badf2ca7a7217:0x1f24b8f61198d350!8m2!3d-22.4870895!4d17.4631457!16zL20vMDd6a2Mx?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{50D57E02-CE7D-4086-BDE0-5961FB898C69}"/>
-    <hyperlink ref="E20" r:id="rId14" display="https://www.google.com/maps/place/%EC%8B%9C%EC%A6%88%EB%A6%AC%EC%97%A0+%EC%BA%A0%ED%94%84%EC%82%AC%EC%9D%B4%ED%8A%B8+-+NWR/@-24.4500775,15.7506268,12z/data=!4m9!3m8!1s0x1c728a898f99a62b:0x2e1eb267fbdbc249!5m2!4m1!1i2!8m2!3d-24.4862708!4d15.7990914!16s%2Fg%2F11cn0qm_4c?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{7B6FC9C3-8F51-42F6-AD33-00DE6263C199}"/>
-    <hyperlink ref="E21" r:id="rId15" xr:uid="{CD9111B8-EA78-457F-93E5-73D21B5D8356}"/>
-    <hyperlink ref="E22" r:id="rId16" display="https://www.google.com/maps/place/%EC%86%8C%EC%84%9C%EC%8A%A4%EB%B8%94%EB%A0%88%EC%9D%B4/@-24.7299883,15.3195806,17z/data=!3m1!4b1!4m6!3m5!1s0x1c720c36bf4379af:0xc1101aae1ad9c253!8m2!3d-24.7299883!4d15.3221555!16s%2Fg%2F1wf4qtjb?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{C9726F3B-461C-4996-B5B1-2045879CD9E6}"/>
-    <hyperlink ref="E23" r:id="rId17" display="https://www.google.com/maps/place/%EB%8D%B0%EB%93%9C%EB%B8%8C%EB%A0%88%EC%9D%B4/@-24.7592732,15.2923894,17z/data=!4m6!3m5!1s0x1c720eb85269ca25:0x91e505d54330767b!8m2!3d-24.7592732!4d15.2923894!16s%2Fm%2F03wbkkh?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{D153F76A-5342-4966-9F4E-7039CAC3EFFB}"/>
-    <hyperlink ref="E24" r:id="rId18" display="https://www.google.com/maps/place/%EC%8B%9C%EC%A6%88%EB%A6%AC%EC%97%A0+%EC%BA%A0%ED%94%84%EC%82%AC%EC%9D%B4%ED%8A%B8+-+NWR/@-24.4500775,15.7506268,12z/data=!4m9!3m8!1s0x1c728a898f99a62b:0x2e1eb267fbdbc249!5m2!4m1!1i2!8m2!3d-24.4862708!4d15.7990914!16s%2Fg%2F11cn0qm_4c?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{BE57540F-46CF-4A8A-BA58-CB578556E112}"/>
-    <hyperlink ref="E26" r:id="rId19" xr:uid="{BF67EE91-A621-4922-8560-9E32325A205B}"/>
-    <hyperlink ref="E25" r:id="rId20" xr:uid="{E16FD79B-BCAC-47DD-B786-5230F7955562}"/>
-    <hyperlink ref="E27" r:id="rId21" display="https://www.google.com/maps/place/%EC%8B%9C%EC%A6%88%EB%A6%AC%EC%97%A0+%EC%BA%A0%ED%94%84%EC%82%AC%EC%9D%B4%ED%8A%B8+-+NWR/@-24.4500775,15.7506268,12z/data=!4m9!3m8!1s0x1c728a898f99a62b:0x2e1eb267fbdbc249!5m2!4m1!1i2!8m2!3d-24.4862708!4d15.7990914!16s%2Fg%2F11cn0qm_4c?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{8E02571A-AD76-4D04-AEAE-91F8982B7CCA}"/>
-    <hyperlink ref="E28" r:id="rId22" xr:uid="{FF0AF7DC-497E-419B-9F68-CE34EC44E922}"/>
-    <hyperlink ref="E29" r:id="rId23" display="https://www.google.com/maps/place/%EB%82%98%EB%AF%B8%EB%B9%84%EC%95%84+%EB%B9%88%ED%8A%B8%ED%9B%84%ED%81%AC/@-22.563751,17.0210266,13z/data=!3m1!4b1!4m6!3m5!1s0x1c0b1b5cb30c01ed:0xe4b84940cc445d3b!8m2!3d-22.5649344!4d17.0842147!16zL20vMGZ0cTc?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{D10D4065-5F67-4E23-8B6E-5C4E78C39A3B}"/>
-    <hyperlink ref="E30" r:id="rId24" display="https://www.google.com/maps/place/Hilton+Garden+Inn+Windhoek/@-22.569885,17.0830968,17z/data=!3m1!4b1!4m9!3m8!1s0x1c0b1b6b8586b239:0xf1a0bbc930def090!5m2!4m1!1i2!8m2!3d-22.569885!4d17.0856717!16s%2Fg%2F11vwm83dz3?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{00A71145-DBE9-438B-8868-7790C10802F8}"/>
-    <hyperlink ref="E31" r:id="rId25" display="https://www.google.com/maps/place/%ED%98%B8%EC%84%B8%EC%95%84+%EC%BF%A0%ED%83%80%EC%BD%94+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@-22.4870895,17.4605708,17z/data=!3m1!4b1!4m6!3m5!1s0x1c0badf2ca7a7217:0x1f24b8f61198d350!8m2!3d-22.4870895!4d17.4631457!16zL20vMDd6a2Mx?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{29F1DAEA-277E-466A-A40C-3FFE02FFD2AF}"/>
-    <hyperlink ref="E32" r:id="rId26" display="https://www.google.com/maps/place/%EC%95%84%EB%94%94%EC%8A%A4%EC%95%84%EB%B0%94%EB%B0%94+%EB%B3%BC%EB%A0%88+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@8.9837932,38.7937261,17z/data=!3m1!4b1!4m6!3m5!1s0x164b858fbf50bd97:0x93a0799b20ab0276!8m2!3d8.9837879!4d38.7963064!16zL20vMDQ3OTc4?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{E4AA03EF-7BBE-460D-8949-AF4516B7AB09}"/>
-    <hyperlink ref="E33" r:id="rId27" display="https://www.google.com/maps/place/%EC%9D%B8%EC%B2%9C%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/data=!3m1!4b1!4m6!3m5!1s0x357b9a833a5efa59:0x8d4ba096cb5cbed4!8m2!3d37.458666!4d126.4419679!16zL20vMDE2MWdi?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{3D8D0619-FED2-4E3C-A6EE-A3EED824D44A}"/>
+    <hyperlink ref="E19" r:id="rId13" display="https://www.google.com/maps/place/%ED%98%B8%EC%84%B8%EC%95%84+%EC%BF%A0%ED%83%80%EC%BD%94+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@-22.4870895,17.4605708,17z/data=!3m1!4b1!4m6!3m5!1s0x1c0badf2ca7a7217:0x1f24b8f61198d350!8m2!3d-22.4870895!4d17.4631457!16zL20vMDd6a2Mx?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{50D57E02-CE7D-4086-BDE0-5961FB898C69}"/>
+    <hyperlink ref="E21" r:id="rId14" display="https://www.google.com/maps/place/%EC%8B%9C%EC%A6%88%EB%A6%AC%EC%97%A0+%EC%BA%A0%ED%94%84%EC%82%AC%EC%9D%B4%ED%8A%B8+-+NWR/@-24.4500775,15.7506268,12z/data=!4m9!3m8!1s0x1c728a898f99a62b:0x2e1eb267fbdbc249!5m2!4m1!1i2!8m2!3d-24.4862708!4d15.7990914!16s%2Fg%2F11cn0qm_4c?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{7B6FC9C3-8F51-42F6-AD33-00DE6263C199}"/>
+    <hyperlink ref="E22" r:id="rId15" xr:uid="{CD9111B8-EA78-457F-93E5-73D21B5D8356}"/>
+    <hyperlink ref="E23" r:id="rId16" display="https://www.google.com/maps/place/%EC%86%8C%EC%84%9C%EC%8A%A4%EB%B8%94%EB%A0%88%EC%9D%B4/@-24.7299883,15.3195806,17z/data=!3m1!4b1!4m6!3m5!1s0x1c720c36bf4379af:0xc1101aae1ad9c253!8m2!3d-24.7299883!4d15.3221555!16s%2Fg%2F1wf4qtjb?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{C9726F3B-461C-4996-B5B1-2045879CD9E6}"/>
+    <hyperlink ref="E24" r:id="rId17" display="https://www.google.com/maps/place/%EB%8D%B0%EB%93%9C%EB%B8%8C%EB%A0%88%EC%9D%B4/@-24.7592732,15.2923894,17z/data=!4m6!3m5!1s0x1c720eb85269ca25:0x91e505d54330767b!8m2!3d-24.7592732!4d15.2923894!16s%2Fm%2F03wbkkh?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{D153F76A-5342-4966-9F4E-7039CAC3EFFB}"/>
+    <hyperlink ref="E25" r:id="rId18" display="https://www.google.com/maps/place/%EC%8B%9C%EC%A6%88%EB%A6%AC%EC%97%A0+%EC%BA%A0%ED%94%84%EC%82%AC%EC%9D%B4%ED%8A%B8+-+NWR/@-24.4500775,15.7506268,12z/data=!4m9!3m8!1s0x1c728a898f99a62b:0x2e1eb267fbdbc249!5m2!4m1!1i2!8m2!3d-24.4862708!4d15.7990914!16s%2Fg%2F11cn0qm_4c?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{BE57540F-46CF-4A8A-BA58-CB578556E112}"/>
+    <hyperlink ref="E27" r:id="rId19" xr:uid="{BF67EE91-A621-4922-8560-9E32325A205B}"/>
+    <hyperlink ref="E26" r:id="rId20" xr:uid="{E16FD79B-BCAC-47DD-B786-5230F7955562}"/>
+    <hyperlink ref="E28" r:id="rId21" display="https://www.google.com/maps/place/%EC%8B%9C%EC%A6%88%EB%A6%AC%EC%97%A0+%EC%BA%A0%ED%94%84%EC%82%AC%EC%9D%B4%ED%8A%B8+-+NWR/@-24.4500775,15.7506268,12z/data=!4m9!3m8!1s0x1c728a898f99a62b:0x2e1eb267fbdbc249!5m2!4m1!1i2!8m2!3d-24.4862708!4d15.7990914!16s%2Fg%2F11cn0qm_4c?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{8E02571A-AD76-4D04-AEAE-91F8982B7CCA}"/>
+    <hyperlink ref="E29" r:id="rId22" xr:uid="{FF0AF7DC-497E-419B-9F68-CE34EC44E922}"/>
+    <hyperlink ref="E30" r:id="rId23" display="https://www.google.com/maps/place/%EB%82%98%EB%AF%B8%EB%B9%84%EC%95%84+%EB%B9%88%ED%8A%B8%ED%9B%84%ED%81%AC/@-22.563751,17.0210266,13z/data=!3m1!4b1!4m6!3m5!1s0x1c0b1b5cb30c01ed:0xe4b84940cc445d3b!8m2!3d-22.5649344!4d17.0842147!16zL20vMGZ0cTc?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{D10D4065-5F67-4E23-8B6E-5C4E78C39A3B}"/>
+    <hyperlink ref="E31" r:id="rId24" display="https://www.google.com/maps/place/Hilton+Garden+Inn+Windhoek/@-22.569885,17.0830968,17z/data=!3m1!4b1!4m9!3m8!1s0x1c0b1b6b8586b239:0xf1a0bbc930def090!5m2!4m1!1i2!8m2!3d-22.569885!4d17.0856717!16s%2Fg%2F11vwm83dz3?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{00A71145-DBE9-438B-8868-7790C10802F8}"/>
+    <hyperlink ref="E32" r:id="rId25" display="https://www.google.com/maps/place/%ED%98%B8%EC%84%B8%EC%95%84+%EC%BF%A0%ED%83%80%EC%BD%94+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@-22.4870895,17.4605708,17z/data=!3m1!4b1!4m6!3m5!1s0x1c0badf2ca7a7217:0x1f24b8f61198d350!8m2!3d-22.4870895!4d17.4631457!16zL20vMDd6a2Mx?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{29F1DAEA-277E-466A-A40C-3FFE02FFD2AF}"/>
+    <hyperlink ref="E33" r:id="rId26" display="https://www.google.com/maps/place/%EC%95%84%EB%94%94%EC%8A%A4%EC%95%84%EB%B0%94%EB%B0%94+%EB%B3%BC%EB%A0%88+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@8.9837932,38.7937261,17z/data=!3m1!4b1!4m6!3m5!1s0x164b858fbf50bd97:0x93a0799b20ab0276!8m2!3d8.9837879!4d38.7963064!16zL20vMDQ3OTc4?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{E4AA03EF-7BBE-460D-8949-AF4516B7AB09}"/>
+    <hyperlink ref="E34" r:id="rId27" display="https://www.google.com/maps/place/%EC%9D%B8%EC%B2%9C%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/data=!3m1!4b1!4m6!3m5!1s0x357b9a833a5efa59:0x8d4ba096cb5cbed4!8m2!3d37.458666!4d126.4419679!16zL20vMDE2MWdi?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{3D8D0619-FED2-4E3C-A6EE-A3EED824D44A}"/>
     <hyperlink ref="E8" r:id="rId28" display="https://www.google.com/maps/place/%EC%84%B8%EB%A0%8C%EC%A7%80%ED%8B%B0+%EA%B5%AD%EB%A6%BD%EA%B3%B5%EC%9B%90/@-2.3188676,34.8236987,13.14z/data=!4m6!3m5!1s0x1832cdd680dac6d1:0x2ea157f39deb3945!8m2!3d-2.3333333!4d34.8333333!16zL20vMGdrM24?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{542A8617-DF23-4039-A526-CCCE0B9271A2}"/>
     <hyperlink ref="E10" r:id="rId29" display="https://www.google.com/maps/place/%EC%84%B8%EB%A0%8C%EC%A7%80%ED%8B%B0+%EA%B5%AD%EB%A6%BD%EA%B3%B5%EC%9B%90/@-2.3188676,34.8236987,13.14z/data=!4m6!3m5!1s0x1832cdd680dac6d1:0x2ea157f39deb3945!8m2!3d-2.3333333!4d34.8333333!16zL20vMGdrM24?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{D23A16AE-A251-41CF-B1FC-19D241B22301}"/>
-    <hyperlink ref="E19" r:id="rId30" xr:uid="{CCB97CBB-F83B-4F4D-8651-7EDD4F5D2BAB}"/>
+    <hyperlink ref="E20" r:id="rId30" xr:uid="{CCB97CBB-F83B-4F4D-8651-7EDD4F5D2BAB}"/>
     <hyperlink ref="E14" r:id="rId31" xr:uid="{0CFAEB2A-9083-469C-ABAD-67395742ABB3}"/>
+    <hyperlink ref="E18" r:id="rId32" display="https://www.google.com/maps/place/O.R.+%ED%83%90%EB%B3%B4+%EA%B5%AD%EC%A0%9C%EA%B3%B5%ED%95%AD/@-26.1393913,28.24422,17z/data=!3m1!4b1!4m6!3m5!1s0x1e95143805a229c3:0xb3bf1c40792821d6!8m2!3d-26.1393913!4d28.2467949!16zL20vMHFuMnY?entry=ttu&amp;g_ep=EgoyMDI0MTEyNC4xIKXMDSoASAFQAw%3D%3D" xr:uid="{4E023887-2661-45E2-B765-15DEAEDF8BEA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId33"/>
 </worksheet>
 </file>
</xml_diff>